<commit_message>
Added plausible maximum and minimum
</commit_message>
<xml_diff>
--- a/data/butterfly brood table-2.xlsx
+++ b/data/butterfly brood table-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsaheywood/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30245424-1D47-0D4C-A514-484351402A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8481396E-7407-654A-9AB2-B1F8C302E4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="162">
   <si>
     <t>Include</t>
   </si>
@@ -516,13 +516,19 @@
   </si>
   <si>
     <t>Spring_before</t>
+  </si>
+  <si>
+    <t>maximum_plausible</t>
+  </si>
+  <si>
+    <t>minimum_plausible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -533,6 +539,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -582,12 +594,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}" name="Table1" displayName="Table1" ref="A1:K210" totalsRowShown="0">
-  <autoFilter ref="A1:K210" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K105">
-    <sortCondition descending="1" ref="C1:C210"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}" name="Table1" displayName="Table1" ref="A1:M210" totalsRowShown="0">
+  <autoFilter ref="A1:M210" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M101">
+    <sortCondition ref="C2:C101"/>
   </sortState>
-  <tableColumns count="11">
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{3601996E-2C3E-8142-BC83-5F7335E5E718}" name="NHM name"/>
     <tableColumn id="2" xr3:uid="{BBF797C0-B981-2543-83B2-6F548250D9DF}" name="Include"/>
     <tableColumn id="3" xr3:uid="{0CE60A84-0487-5147-94CC-D0076335687C}" name="Univoltine"/>
@@ -599,6 +611,8 @@
     <tableColumn id="9" xr3:uid="{D90C879A-52CE-4927-8ECE-385F90637BA5}" name="Brood1Use"/>
     <tableColumn id="10" xr3:uid="{6C2BB67C-CEEC-4860-98DE-976E90F4F5BB}" name="Brood2Use"/>
     <tableColumn id="11" xr3:uid="{EAAA7C43-5B70-48BA-ABBD-B9AFF6AC64AF}" name="FirstMonthBrood2"/>
+    <tableColumn id="12" xr3:uid="{A7A58695-6D6E-FB4E-95B9-F4D9E68F1832}" name="maximum_plausible"/>
+    <tableColumn id="13" xr3:uid="{5B19093F-47AF-6046-A900-01BE4EA41468}" name="minimum_plausible"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A24936-E824-B74E-933F-86465AE8095B}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,9 +951,11 @@
     <col min="8" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -973,360 +989,516 @@
       <c r="K1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>24</v>
+      </c>
+      <c r="M2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
         <v>113</v>
       </c>
-      <c r="I2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>14</v>
+      </c>
+      <c r="M3">
         <v>9</v>
       </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" t="s">
-        <v>154</v>
-      </c>
-      <c r="K3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" t="s">
         <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>118</v>
       </c>
       <c r="I4" t="s">
         <v>155</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
-      </c>
-      <c r="K4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>17</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
       </c>
       <c r="I5" t="s">
         <v>155</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
-      </c>
-      <c r="K5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H6" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
-        <v>154</v>
-      </c>
-      <c r="K6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>23</v>
+      </c>
+      <c r="M6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" t="s">
-        <v>120</v>
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>109</v>
       </c>
       <c r="I7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s">
+        <v>146</v>
       </c>
       <c r="I8" t="s">
         <v>155</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
         <v>119</v>
       </c>
+      <c r="G9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="I9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
-      </c>
-      <c r="K9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" t="s">
+        <v>155</v>
+      </c>
+      <c r="J10" t="s">
+        <v>156</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>33</v>
+      </c>
+      <c r="M10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>24</v>
+      </c>
+      <c r="M11">
         <v>18</v>
       </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" t="s">
-        <v>157</v>
-      </c>
-      <c r="J10" t="s">
-        <v>154</v>
-      </c>
-      <c r="K10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J11" t="s">
-        <v>154</v>
-      </c>
-      <c r="K11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>114</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>154</v>
-      </c>
-      <c r="K12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>25</v>
+      </c>
+      <c r="M12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" t="s">
-        <v>105</v>
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>126</v>
       </c>
       <c r="I13" t="s">
         <v>155</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>26</v>
+      </c>
+      <c r="M13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
         <v>113</v>
       </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" t="s">
+        <v>120</v>
+      </c>
       <c r="I14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
-      </c>
-      <c r="K14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>17</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -1335,13 +1507,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s">
         <v>157</v>
@@ -1352,10 +1521,16 @@
       <c r="K15" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -1364,13 +1539,13 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J16" t="s">
         <v>154</v>
@@ -1378,10 +1553,16 @@
       <c r="K16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>40</v>
+      </c>
+      <c r="M16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1390,10 +1571,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H17" t="s">
         <v>120</v>
@@ -1407,10 +1588,16 @@
       <c r="K17" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>26</v>
+      </c>
+      <c r="M17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -1422,10 +1609,10 @@
         <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="I18" t="s">
         <v>157</v>
@@ -1437,9 +1624,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -1448,16 +1635,13 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H19" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="I19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J19" t="s">
         <v>154</v>
@@ -1465,10 +1649,16 @@
       <c r="K19" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>33</v>
+      </c>
+      <c r="M19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -1477,16 +1667,13 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
-      </c>
-      <c r="H20" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J20" t="s">
         <v>154</v>
@@ -1494,10 +1681,16 @@
       <c r="K20" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>33</v>
+      </c>
+      <c r="M20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1511,6 +1704,9 @@
       <c r="E21" t="s">
         <v>129</v>
       </c>
+      <c r="H21" t="s">
+        <v>120</v>
+      </c>
       <c r="I21" t="s">
         <v>157</v>
       </c>
@@ -1520,10 +1716,16 @@
       <c r="K21" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>37</v>
+      </c>
+      <c r="M21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -1535,10 +1737,10 @@
         <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="I22" t="s">
         <v>157</v>
@@ -1550,9 +1752,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -1561,10 +1763,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>128</v>
+      </c>
+      <c r="H23" t="s">
+        <v>120</v>
       </c>
       <c r="I23" t="s">
         <v>157</v>
@@ -1575,10 +1780,16 @@
       <c r="K23" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>23</v>
+      </c>
+      <c r="M23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1587,10 +1798,13 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>121</v>
+      </c>
+      <c r="H24" t="s">
+        <v>120</v>
       </c>
       <c r="I24" t="s">
         <v>157</v>
@@ -1601,10 +1815,16 @@
       <c r="K24" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>24</v>
+      </c>
+      <c r="M24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -1613,10 +1833,10 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="I25" t="s">
         <v>158</v>
@@ -1627,10 +1847,16 @@
       <c r="K25" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>16</v>
+      </c>
+      <c r="M25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -1639,16 +1865,13 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
-      </c>
-      <c r="H26" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J26" t="s">
         <v>154</v>
@@ -1656,10 +1879,16 @@
       <c r="K26" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>14</v>
+      </c>
+      <c r="M26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -1668,16 +1897,13 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="I27" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J27" t="s">
         <v>154</v>
@@ -1685,10 +1911,16 @@
       <c r="K27" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>20</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -1697,10 +1929,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H28" t="s">
         <v>120</v>
@@ -1714,10 +1946,16 @@
       <c r="K28" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>20</v>
+      </c>
+      <c r="M28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -1726,10 +1964,10 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="I29" t="s">
         <v>157</v>
@@ -1740,10 +1978,16 @@
       <c r="K29" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>13</v>
+      </c>
+      <c r="M29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -1752,14 +1996,11 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
         <v>129</v>
       </c>
-      <c r="H30" t="s">
-        <v>120</v>
-      </c>
       <c r="I30" t="s">
         <v>157</v>
       </c>
@@ -1770,9 +2011,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1781,13 +2022,13 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J31" t="s">
         <v>154</v>
@@ -1796,9 +2037,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -1807,13 +2048,16 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="H32" t="s">
+        <v>120</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J32" t="s">
         <v>154</v>
@@ -1821,10 +2065,16 @@
       <c r="K32" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>14</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -1836,36 +2086,42 @@
         <v>113</v>
       </c>
       <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="I33" t="s">
+        <v>157</v>
+      </c>
+      <c r="J33" t="s">
+        <v>154</v>
+      </c>
+      <c r="K33" t="s">
+        <v>154</v>
+      </c>
+      <c r="L33">
+        <v>24</v>
+      </c>
+      <c r="M33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>135</v>
       </c>
-      <c r="I33" t="s">
-        <v>155</v>
-      </c>
-      <c r="J33" t="s">
-        <v>154</v>
-      </c>
-      <c r="K33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>119</v>
-      </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J34" t="s">
         <v>154</v>
@@ -1873,10 +2129,16 @@
       <c r="K34" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>32</v>
+      </c>
+      <c r="M34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -1885,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E35" t="s">
         <v>113</v>
@@ -1899,10 +2161,16 @@
       <c r="K35" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>15</v>
+      </c>
+      <c r="M35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -1911,16 +2179,16 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H36" t="s">
         <v>108</v>
       </c>
       <c r="I36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J36" t="s">
         <v>154</v>
@@ -1928,10 +2196,16 @@
       <c r="K36" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>16</v>
+      </c>
+      <c r="M36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -1940,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
         <v>129</v>
@@ -1949,63 +2223,69 @@
         <v>120</v>
       </c>
       <c r="I37" t="s">
+        <v>157</v>
+      </c>
+      <c r="J37" t="s">
+        <v>154</v>
+      </c>
+      <c r="K37" t="s">
+        <v>154</v>
+      </c>
+      <c r="L37">
+        <v>34</v>
+      </c>
+      <c r="M37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" t="s">
         <v>158</v>
       </c>
-      <c r="J37" t="s">
-        <v>154</v>
-      </c>
-      <c r="K37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="J38" t="s">
+        <v>154</v>
+      </c>
+      <c r="K38" t="s">
+        <v>154</v>
+      </c>
+      <c r="L38">
+        <v>34</v>
+      </c>
+      <c r="M38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
         <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>133</v>
-      </c>
-      <c r="H38" t="s">
-        <v>120</v>
-      </c>
-      <c r="I38" t="s">
-        <v>157</v>
-      </c>
-      <c r="J38" t="s">
-        <v>154</v>
-      </c>
-      <c r="K38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" t="b">
-        <v>1</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>147</v>
       </c>
       <c r="E39" t="s">
         <v>133</v>
       </c>
-      <c r="H39" t="s">
-        <v>120</v>
-      </c>
       <c r="I39" t="s">
         <v>157</v>
       </c>
@@ -2015,10 +2295,16 @@
       <c r="K39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>33</v>
+      </c>
+      <c r="M39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -2027,53 +2313,65 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E40" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="I40" t="s">
+        <v>155</v>
+      </c>
+      <c r="J40" t="s">
+        <v>154</v>
+      </c>
+      <c r="K40" t="s">
+        <v>154</v>
+      </c>
+      <c r="L40">
+        <v>20</v>
+      </c>
+      <c r="M40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" t="s">
+        <v>133</v>
+      </c>
+      <c r="H41" t="s">
+        <v>120</v>
+      </c>
+      <c r="I41" t="s">
         <v>157</v>
       </c>
-      <c r="J40" t="s">
-        <v>154</v>
-      </c>
-      <c r="K40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" t="s">
-        <v>130</v>
-      </c>
-      <c r="H41" t="s">
-        <v>108</v>
-      </c>
-      <c r="I41" t="s">
-        <v>155</v>
-      </c>
       <c r="J41" t="s">
         <v>154</v>
       </c>
       <c r="K41" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>30</v>
+      </c>
+      <c r="M41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -2085,10 +2383,7 @@
         <v>119</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I42" t="s">
         <v>157</v>
@@ -2099,243 +2394,255 @@
       <c r="K42" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>30</v>
+      </c>
+      <c r="M42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
       </c>
       <c r="C43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E43" t="s">
-        <v>115</v>
-      </c>
-      <c r="F43" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="I43" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J43" t="s">
-        <v>156</v>
-      </c>
-      <c r="K43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K43" t="s">
+        <v>154</v>
+      </c>
+      <c r="L43">
+        <v>23</v>
+      </c>
+      <c r="M43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
       </c>
       <c r="C44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E44" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" t="s">
-        <v>102</v>
-      </c>
-      <c r="G44" t="s">
-        <v>119</v>
+        <v>128</v>
+      </c>
+      <c r="H44" t="s">
+        <v>120</v>
       </c>
       <c r="I44" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J44" t="s">
-        <v>156</v>
-      </c>
-      <c r="K44">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K44" t="s">
+        <v>154</v>
+      </c>
+      <c r="L44">
+        <v>23</v>
+      </c>
+      <c r="M44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
       </c>
       <c r="C45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" t="s">
-        <v>109</v>
-      </c>
-      <c r="G45" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="I45" t="s">
         <v>155</v>
       </c>
       <c r="J45" t="s">
-        <v>156</v>
-      </c>
-      <c r="K45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K45" t="s">
+        <v>154</v>
+      </c>
+      <c r="L45">
+        <v>18</v>
+      </c>
+      <c r="M45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
       </c>
       <c r="C46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" t="s">
         <v>114</v>
-      </c>
-      <c r="E46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" t="s">
-        <v>109</v>
-      </c>
-      <c r="G46" t="s">
-        <v>109</v>
       </c>
       <c r="I46" t="s">
         <v>155</v>
       </c>
       <c r="J46" t="s">
-        <v>156</v>
-      </c>
-      <c r="K46">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K46" t="s">
+        <v>154</v>
+      </c>
+      <c r="L46">
+        <v>35</v>
+      </c>
+      <c r="M46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
       </c>
       <c r="C47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E47" t="s">
-        <v>131</v>
-      </c>
-      <c r="F47" t="s">
-        <v>126</v>
-      </c>
-      <c r="G47" t="s">
-        <v>109</v>
+        <v>132</v>
+      </c>
+      <c r="H47" t="s">
+        <v>120</v>
       </c>
       <c r="I47" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J47" t="s">
-        <v>156</v>
-      </c>
-      <c r="K47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K47" t="s">
+        <v>154</v>
+      </c>
+      <c r="L47">
+        <v>17</v>
+      </c>
+      <c r="M47">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
       </c>
       <c r="C48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E48" t="s">
         <v>113</v>
       </c>
-      <c r="F48" t="s">
-        <v>104</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
-      </c>
       <c r="I48" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J48" t="s">
-        <v>156</v>
-      </c>
-      <c r="K48">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K48" t="s">
+        <v>154</v>
+      </c>
+      <c r="L48">
+        <v>45</v>
+      </c>
+      <c r="M48">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
       </c>
       <c r="C49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F49" t="s">
-        <v>109</v>
-      </c>
-      <c r="G49" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H49" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="I49" t="s">
         <v>155</v>
       </c>
       <c r="J49" t="s">
-        <v>156</v>
-      </c>
-      <c r="K49">
+        <v>154</v>
+      </c>
+      <c r="K49" t="s">
+        <v>154</v>
+      </c>
+      <c r="L49">
+        <v>20</v>
+      </c>
+      <c r="M49">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
       </c>
       <c r="C50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
         <v>131</v>
@@ -2343,164 +2650,200 @@
       <c r="E50" t="s">
         <v>113</v>
       </c>
-      <c r="F50" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" t="s">
-        <v>134</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J50" t="s">
+        <v>154</v>
+      </c>
+      <c r="K50" t="s">
+        <v>154</v>
+      </c>
+      <c r="L50">
+        <v>12</v>
+      </c>
+      <c r="M50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" t="s">
+        <v>129</v>
+      </c>
+      <c r="H51" t="s">
         <v>120</v>
       </c>
-      <c r="I50" t="s">
-        <v>155</v>
-      </c>
-      <c r="J50" t="s">
-        <v>156</v>
-      </c>
-      <c r="K50">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" t="s">
-        <v>113</v>
-      </c>
-      <c r="E51" t="s">
-        <v>119</v>
-      </c>
-      <c r="H51" t="s">
-        <v>107</v>
-      </c>
       <c r="I51" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J51" t="s">
-        <v>156</v>
-      </c>
-      <c r="K51">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K51" t="s">
+        <v>154</v>
+      </c>
+      <c r="L51">
+        <v>23</v>
+      </c>
+      <c r="M51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
       </c>
       <c r="C52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="H52" t="s">
+        <v>105</v>
       </c>
       <c r="I52" t="s">
         <v>155</v>
       </c>
       <c r="J52" t="s">
-        <v>156</v>
-      </c>
-      <c r="K52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K52" t="s">
+        <v>154</v>
+      </c>
+      <c r="L52">
+        <v>17</v>
+      </c>
+      <c r="M52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
       </c>
       <c r="C53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="E53" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" t="s">
-        <v>119</v>
-      </c>
-      <c r="G53" t="s">
-        <v>109</v>
+        <v>130</v>
+      </c>
+      <c r="H53" t="s">
+        <v>108</v>
       </c>
       <c r="I53" t="s">
         <v>155</v>
       </c>
       <c r="J53" t="s">
-        <v>156</v>
-      </c>
-      <c r="K53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K53" t="s">
+        <v>154</v>
+      </c>
+      <c r="L53">
+        <v>17</v>
+      </c>
+      <c r="M53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
       </c>
       <c r="C54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
-        <v>145</v>
-      </c>
-      <c r="F54" t="s">
-        <v>144</v>
-      </c>
-      <c r="G54" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="H54" t="s">
+        <v>108</v>
       </c>
       <c r="I54" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J54" t="s">
-        <v>156</v>
-      </c>
-      <c r="K54">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K54" t="s">
+        <v>154</v>
+      </c>
+      <c r="L54">
+        <v>19</v>
+      </c>
+      <c r="M54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="B55" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" t="s">
+        <v>133</v>
       </c>
       <c r="H55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="I55" t="s">
+        <v>157</v>
+      </c>
+      <c r="J55" t="s">
+        <v>154</v>
+      </c>
+      <c r="K55" t="s">
+        <v>154</v>
+      </c>
+      <c r="L55">
+        <v>13</v>
+      </c>
+      <c r="M55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
@@ -2509,10 +2852,10 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I56" t="s">
         <v>155</v>
@@ -2523,111 +2866,99 @@
       <c r="K56" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>15</v>
+      </c>
+      <c r="M56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
       </c>
       <c r="C57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E57" t="s">
-        <v>114</v>
-      </c>
-      <c r="F57" t="s">
-        <v>119</v>
-      </c>
-      <c r="G57" t="s">
-        <v>119</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>157</v>
+        <v>129</v>
+      </c>
+      <c r="H57" t="s">
+        <v>120</v>
       </c>
       <c r="I57" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J57" t="s">
-        <v>156</v>
-      </c>
-      <c r="K57">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="K57" t="s">
+        <v>154</v>
+      </c>
+      <c r="L57">
+        <v>14</v>
+      </c>
+      <c r="M57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B58" t="b">
-        <v>1</v>
-      </c>
-      <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>125</v>
-      </c>
-      <c r="E58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I58" t="s">
-        <v>157</v>
-      </c>
-      <c r="J58" t="s">
-        <v>154</v>
-      </c>
-      <c r="K58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
@@ -2635,7 +2966,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="B65" t="b">
         <v>0</v>
@@ -2643,7 +2974,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B66" t="b">
         <v>0</v>
@@ -2651,7 +2982,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
@@ -2659,7 +2990,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B68" t="b">
         <v>0</v>
@@ -2667,7 +2998,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B69" t="b">
         <v>0</v>
@@ -2675,7 +3006,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B70" t="b">
         <v>0</v>
@@ -2683,7 +3014,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B71" t="b">
         <v>0</v>
@@ -2691,7 +3022,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B72" t="b">
         <v>0</v>
@@ -2699,7 +3030,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B73" t="b">
         <v>0</v>
@@ -2707,7 +3038,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B74" t="b">
         <v>0</v>
@@ -2715,7 +3046,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B75" t="b">
         <v>0</v>
@@ -2723,7 +3054,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B76" t="b">
         <v>0</v>
@@ -2731,7 +3062,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B77" t="b">
         <v>0</v>
@@ -2739,7 +3070,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B78" t="b">
         <v>0</v>
@@ -2747,7 +3078,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B79" t="b">
         <v>0</v>
@@ -2755,135 +3086,138 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="B80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>54</v>
+      </c>
+      <c r="B84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>85</v>
       </c>
-      <c r="B81" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="B89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>94</v>
       </c>
-      <c r="B82" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>95</v>
-      </c>
-      <c r="B83" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>96</v>
-      </c>
-      <c r="B84" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>99</v>
-      </c>
-      <c r="B87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>101</v>
-      </c>
-      <c r="B88" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>14</v>
-      </c>
-      <c r="B89" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>30</v>
-      </c>
-      <c r="B91" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>37</v>
-      </c>
-      <c r="B92" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>38</v>
-      </c>
-      <c r="B93" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>45</v>
-      </c>
-      <c r="B94" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>48</v>
-      </c>
       <c r="B95" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B96" t="b">
         <v>0</v>
@@ -2891,7 +3225,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B97" t="b">
         <v>0</v>
@@ -2899,7 +3233,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B98" t="b">
         <v>0</v>
@@ -2907,7 +3241,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="B99" t="b">
         <v>0</v>
@@ -2915,7 +3249,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B100" t="b">
         <v>0</v>
@@ -2923,13 +3257,14 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B101" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Create brood_table csv.  Plot max,min on distributions
</commit_message>
<xml_diff>
--- a/data/butterfly brood table-2.xlsx
+++ b/data/butterfly brood table-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsaheywood/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\Butterfly_Project_MBiol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8481396E-7407-654A-9AB2-B1F8C302E4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6313858C-9EB5-467C-A7DB-7DDDB8FAECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="162">
   <si>
     <t>Include</t>
   </si>
@@ -528,17 +528,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -570,12 +563,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,11 +929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A24936-E824-B74E-933F-86465AE8095B}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
@@ -955,7 +947,7 @@
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -996,7 +988,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1034,7 +1026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1075,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1113,7 +1105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1151,7 +1143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1186,7 +1178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1224,7 +1216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1262,7 +1254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -1284,9 +1276,6 @@
       <c r="G9" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="I9" t="s">
         <v>155</v>
       </c>
@@ -1303,7 +1292,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1341,7 +1330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1379,7 +1368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1417,7 +1406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1455,7 +1444,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1496,7 +1485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1528,7 +1517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1560,7 +1549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -1595,7 +1584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1624,7 +1613,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1656,7 +1645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1688,7 +1677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1723,7 +1712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -1752,7 +1741,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1787,7 +1776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1822,7 +1811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1854,7 +1843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -1886,7 +1875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1918,7 +1907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1953,7 +1942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1985,7 +1974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2011,7 +2000,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2037,7 +2026,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2072,7 +2061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2104,7 +2093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2136,7 +2125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2168,7 +2157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -2203,7 +2192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -2238,7 +2227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2270,7 +2259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -2302,7 +2291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2334,7 +2323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2369,7 +2358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -2401,7 +2390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2433,7 +2422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2468,7 +2457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2500,7 +2489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2532,7 +2521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -2567,7 +2556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2599,7 +2588,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2634,7 +2623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -2666,7 +2655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2701,7 +2690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>21</v>
       </c>
@@ -2736,7 +2725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -2771,7 +2760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -2806,7 +2795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2841,7 +2830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2873,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -2908,7 +2897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2916,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2924,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2932,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -2940,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -2948,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2956,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -2964,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -2972,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -2980,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -2988,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -2996,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -3004,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3012,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>27</v>
       </c>
@@ -3020,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -3028,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -3036,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>53</v>
       </c>
@@ -3044,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -3052,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -3060,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -3068,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -3076,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>99</v>
       </c>
@@ -3084,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -3092,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -3100,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>45</v>
       </c>
@@ -3108,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -3116,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>54</v>
       </c>
@@ -3124,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>71</v>
       </c>
@@ -3132,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>29</v>
       </c>
@@ -3140,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>49</v>
       </c>
@@ -3148,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -3159,7 +3148,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -3167,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -3175,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -3183,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -3191,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>25</v>
       </c>
@@ -3199,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>67</v>
       </c>
@@ -3207,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -3215,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>70</v>
       </c>
@@ -3223,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3231,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>84</v>
       </c>
@@ -3239,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -3247,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -3255,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>38</v>
       </c>
@@ -3264,7 +3253,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>